<commit_message>
Updated Excel file statistics & added console app image
</commit_message>
<xml_diff>
--- a/GenAICreateQuestionsFromParagraphs/SampleResults/macOS/sampleDurationResults.xlsx
+++ b/GenAICreateQuestionsFromParagraphs/SampleResults/macOS/sampleDurationResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bczernicki\source\repos\GenAICreateQuestionsFromParagraphs\GenAICreateQuestionsFromParagraphs\SampleResults\macOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041C03E-6575-4D21-AE56-A8C545FCF54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10684C-1F81-4A66-B5C9-5892262C05F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22875" windowHeight="13650" xr2:uid="{3D69E190-3EF2-754E-8869-F8FDD486E5BF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22875" windowHeight="13650" activeTab="1" xr2:uid="{3D69E190-3EF2-754E-8869-F8FDD486E5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
   <si>
     <t>gpt-35-turbo-1106</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Median</t>
-  </si>
-  <si>
-    <t>Mode</t>
   </si>
   <si>
     <t>Standard Deviation</t>
@@ -119,7 +116,13 @@
     <t>gpt-4-1106-preview-payg</t>
   </si>
   <si>
-    <t>Sum (time of job)</t>
+    <t>gpt-35-turbo-1106-payg-P90</t>
+  </si>
+  <si>
+    <t>P90</t>
+  </si>
+  <si>
+    <t>Sum (of 100 requests)</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -231,11 +234,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,6 +400,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,302 +529,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="11"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="15"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="16"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="17"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="18"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="20"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000010-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="21"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000011-BACA-44A1-818E-C9D2ABF8370E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>'GPT-4'!$A$2:$A$27</c:f>
@@ -777,34 +629,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -816,25 +668,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1097,6 +949,194 @@
           </c:ext>
         </c:extLst>
       </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GPT-4'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="548640" rIns="38100" bIns="0" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-ED47-40E5-BBF4-3CBD678E2E04}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="548640" rIns="38100" bIns="0" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="0.25"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GPT-4'!$E$2:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="17">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ED47-40E5-BBF4-3CBD678E2E04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1385237040"/>
+        <c:axId val="1385235600"/>
+      </c:scatterChart>
       <c:catAx>
         <c:axId val="1385237040"/>
         <c:scaling>
@@ -1169,7 +1209,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1214,6 +1254,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1371,7 +1415,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'GPT-4'!$E$1</c:f>
+              <c:f>'GPT-4'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1392,152 +1436,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-06AE-4395-9E7B-0341D2E370EE}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-06AE-4395-9E7B-0341D2E370EE}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-06AE-4395-9E7B-0341D2E370EE}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-06AE-4395-9E7B-0341D2E370EE}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-06AE-4395-9E7B-0341D2E370EE}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-06AE-4395-9E7B-0341D2E370EE}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>'GPT-4'!$A$2:$A$27</c:f>
@@ -1627,7 +1525,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'GPT-4'!$E$1:$E$27</c:f>
+              <c:f>'GPT-4'!$F$1:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -1638,22 +1536,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1944,6 +1842,153 @@
           </c:ext>
         </c:extLst>
       </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GPT-4'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="0" rIns="38100" bIns="0" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="0.60000000000000009"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GPT-4'!$G$2:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CAE5-441B-B402-C12B0BAF4312}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1089246207"/>
+        <c:axId val="1089245247"/>
+      </c:scatterChart>
       <c:catAx>
         <c:axId val="1089246207"/>
         <c:scaling>
@@ -2016,7 +2061,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2061,6 +2106,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2148,36 +2197,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2751,6 +2770,132 @@
           </c:ext>
         </c:extLst>
       </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'GPT3-5'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gpt-35-turbo-1106-payg-P90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="1"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GPT3-5'!$G$2:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-05F6-4378-BEFC-E51F4C3CAE8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1400420224"/>
+        <c:axId val="1400418304"/>
+      </c:scatterChart>
       <c:catAx>
         <c:axId val="1400420224"/>
         <c:scaling>
@@ -2868,6 +3013,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2938,6 +3087,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2997,7 +3147,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'GPT3-5'!$G$1</c:f>
+              <c:f>'GPT3-5'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3137,7 +3287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'GPT3-5'!$G$2:$G$37</c:f>
+              <c:f>'GPT3-5'!$H$2:$H$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -7436,13 +7586,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>707486</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>84935</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>262986</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>122611</xdr:rowOff>
@@ -7472,13 +7622,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>703252</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>148955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>258752</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>186632</xdr:rowOff>
@@ -7513,14 +7663,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3401</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>363991</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>23130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>183696</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>102051</xdr:rowOff>
     </xdr:to>
@@ -7549,14 +7699,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3399</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>363989</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>2720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>183695</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>176891</xdr:rowOff>
     </xdr:to>
@@ -7587,6 +7737,53 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.50869</cdr:x>
+      <cdr:y>0.04479</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.6453</cdr:x>
+      <cdr:y>0.11415</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B2B7C33-B129-8C4B-8687-3815C3E6E6F8}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2888116" y="153763"/>
+          <a:ext cx="775608" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>P90</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7964,15 +8161,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202A859E-2170-114F-A3C6-EFC3AA41D3AC}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.8125" customWidth="1"/>
+    <col min="1" max="1" width="18.4375" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="17.3125" customWidth="1"/>
     <col min="4" max="4" width="13.3125" customWidth="1"/>
@@ -7993,15 +8190,15 @@
       </c>
       <c r="D1" s="6"/>
       <c r="F1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" s="6"/>
       <c r="K1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" s="6"/>
     </row>
@@ -8103,68 +8300,68 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="10">
+        <v>0.49482220634694851</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="10">
+        <v>0.41291690813592125</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="G6" s="10">
+        <v>4.43934904477545</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="9" t="e">
-        <v>#N/A</v>
+      <c r="I6" s="10">
+        <v>1.1249625690260856</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
       </c>
-      <c r="L6" t="e">
-        <v>#N/A</v>
+      <c r="L6">
+        <v>1.4972164240436201</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10">
-        <v>0.49482220634694851</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="9">
+        <v>0.24484901589406208</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10">
-        <v>0.41291690813592125</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="9">
+        <v>0.17050037302452883</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="10">
-        <v>4.43934904477545</v>
-      </c>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="9">
+        <v>19.707819941348703</v>
+      </c>
+      <c r="H7" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="10">
-        <v>1.1249625690260856</v>
+      <c r="I7" s="9">
+        <v>1.2655407817097704</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
       </c>
       <c r="L7">
-        <v>1.4972164240436201</v>
+        <v>2.2416570204259654</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -8172,31 +8369,31 @@
         <v>9</v>
       </c>
       <c r="B8" s="9">
-        <v>0.24484901589406208</v>
+        <v>0.52231307898131218</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="9">
-        <v>0.17050037302452883</v>
+        <v>-0.56434713680001058</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="9">
-        <v>19.707819941348703</v>
+        <v>1.9137587949976269</v>
       </c>
       <c r="H8" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="9">
-        <v>1.2655407817097704</v>
+        <v>2.6137852855512755</v>
       </c>
       <c r="K8" t="s">
         <v>9</v>
       </c>
       <c r="L8">
-        <v>2.2416570204259654</v>
+        <v>8.5842757882989531</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -8204,31 +8401,31 @@
         <v>10</v>
       </c>
       <c r="B9" s="9">
-        <v>0.52231307898131218</v>
+        <v>0.81305124684382379</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="9">
-        <v>-0.56434713680001058</v>
+        <v>0.1134860912327932</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="9">
-        <v>1.9137587949976269</v>
+        <v>1.5260927977788079</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="9">
-        <v>2.6137852855512755</v>
+        <v>1.5687206987834401</v>
       </c>
       <c r="K9" t="s">
         <v>10</v>
       </c>
       <c r="L9">
-        <v>8.5842757882989531</v>
+        <v>2.3616290678074181</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -8236,63 +8433,64 @@
         <v>11</v>
       </c>
       <c r="B10" s="9">
-        <v>0.81305124684382379</v>
+        <v>2.3989515999999997</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="9">
-        <v>0.1134860912327932</v>
+        <v>1.8945508000000002</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="9">
-        <v>1.5260927977788079</v>
+        <v>19.2430789</v>
       </c>
       <c r="H10" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="9">
-        <v>1.5687206987834401</v>
+        <v>5.5489025999999999</v>
       </c>
       <c r="K10" t="s">
         <v>11</v>
       </c>
       <c r="L10">
-        <v>2.3616290678074181</v>
+        <v>12.063437499999999</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9">
-        <v>2.3989515999999997</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="10">
+        <v>0.43290729999999999</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="9">
-        <v>1.8945508000000002</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="D11" s="10">
+        <v>0.2110523</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="9">
-        <v>19.2430789</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G11" s="10">
+        <v>1.6614438</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="9">
-        <v>5.5489025999999999</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" s="10">
+        <v>0.75761449999999997</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L11">
-        <v>12.063437499999999</v>
+      <c r="L11" s="7">
+        <v>0.80460739999999997</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -8300,128 +8498,95 @@
         <v>13</v>
       </c>
       <c r="B12" s="10">
-        <v>0.43290729999999999</v>
+        <v>2.8318588999999998</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="10">
-        <v>0.2110523</v>
+        <v>2.1056031000000002</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="10">
-        <v>1.6614438</v>
+        <v>20.904522700000001</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="10">
-        <v>0.75761449999999997</v>
+        <v>6.3065170999999998</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="L12" s="7">
-        <v>0.80460739999999997</v>
+        <v>12.868044899999999</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="7" t="s">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9">
+        <v>114.20632749999996</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="9">
+        <v>100.21668220000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="9">
+        <v>621.7139024999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="9">
+        <v>250.89265569999992</v>
+      </c>
+      <c r="K13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10">
-        <v>2.8318588999999998</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="10">
-        <v>2.1056031000000002</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="10">
-        <v>20.904522700000001</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="10">
-        <v>6.3065170999999998</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="7">
-        <v>12.868044899999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="9">
-        <v>114.20632749999996</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="9">
-        <v>100.21668220000001</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="9">
-        <v>621.7139024999999</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="9">
-        <v>250.89265569999992</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="L13">
+        <v>1073.4370789999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16.149999999999999" thickBot="1">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L14">
-        <v>1073.4370789999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="16.149999999999999" thickBot="1">
-      <c r="A15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5">
+      <c r="B14" s="5">
         <v>100</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5">
         <v>100</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="5">
+      <c r="F14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="5">
         <v>100</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="H14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="5">
         <v>100</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="5">
+      <c r="K14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="5">
         <v>400</v>
       </c>
     </row>
@@ -8432,38 +8597,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E6C42B-7D81-C345-B5B5-08C788A006F8}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="25.5625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.3125" customWidth="1"/>
-    <col min="4" max="4" width="30.625" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="4" max="5" width="30.625" customWidth="1"/>
+    <col min="6" max="7" width="27" customWidth="1"/>
+    <col min="8" max="14" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:14">
       <c r="A1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8474,15 +8653,22 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f>COUNTIF(B:B, A2)</f>
+        <f>COUNTIF(B:B, A2)/100</f>
         <v>0</v>
       </c>
-      <c r="E2">
-        <f>COUNTIF(C:C, A2)</f>
+      <c r="F2">
+        <f>COUNTIF(C:C, A2)/100</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="20"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8493,15 +8679,22 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f>COUNTIF(B:B, A3)</f>
+        <f t="shared" ref="D3:D27" si="0">COUNTIF(B:B, A3)/100</f>
         <v>0</v>
       </c>
-      <c r="E3">
-        <f>COUNTIF(C:C, A3)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <f t="shared" ref="F3:F27" si="1">COUNTIF(C:C, A3)/100</f>
+        <v>0.09</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8512,15 +8705,22 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D27" si="0">COUNTIF(B:B, A4)</f>
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E27" si="1">COUNTIF(C:C, A4)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="20"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8532,14 +8732,21 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="E5">
+        <v>0.21</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0.22</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="20"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8551,14 +8758,21 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="E6">
+        <v>0.16</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="20"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8570,14 +8784,24 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E7">
+        <v>0.06</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.03</v>
+      </c>
+      <c r="G7">
+        <v>0.65</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8589,14 +8813,21 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E8">
+        <v>0.09</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.04</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="20"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8608,14 +8839,21 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E9">
+        <v>0.06</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8627,14 +8865,21 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E10">
+        <v>0.04</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="H10" s="18"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="20"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8646,14 +8891,21 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="E11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="H11" s="18"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="20"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8665,14 +8917,21 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E12">
+        <v>0.04</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>11</v>
       </c>
@@ -8684,14 +8943,21 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E13">
+        <v>0.04</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="H13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8705,12 +8971,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="H14" s="18"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8724,12 +8997,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="H15" s="18"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8743,12 +9023,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="H16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="20"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>15</v>
       </c>
@@ -8760,14 +9047,21 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="20"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>16</v>
       </c>
@@ -8779,14 +9073,21 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E18">
+        <v>0.02</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18" s="18"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="20"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>17</v>
       </c>
@@ -8798,14 +9099,24 @@
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="E19">
+        <v>0.25</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="20"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>18</v>
       </c>
@@ -8817,14 +9128,21 @@
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E20">
+        <v>0.02</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="H20" s="18"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>19</v>
       </c>
@@ -8838,12 +9156,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="H21" s="18"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="20"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>20</v>
       </c>
@@ -8855,14 +9180,21 @@
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E22">
+        <v>0.01</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="20"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23">
         <v>21</v>
       </c>
@@ -8874,14 +9206,21 @@
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23">
+        <v>0.01</v>
+      </c>
+      <c r="F23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="H23" s="18"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="20"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24">
         <v>22</v>
       </c>
@@ -8895,12 +9234,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="20"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>23</v>
       </c>
@@ -8914,12 +9260,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="20"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26">
         <v>24</v>
       </c>
@@ -8933,12 +9286,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="H26" s="18"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="20"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27">
         <v>25</v>
       </c>
@@ -8952,36 +9312,67 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="H27" s="18"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="20"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="H28" s="18"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="20"/>
+    </row>
+    <row r="29" spans="1:14">
       <c r="B29" s="1">
         <v>3</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="20"/>
+    </row>
+    <row r="30" spans="1:14">
       <c r="B30" s="1">
         <v>4</v>
       </c>
       <c r="C30" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="H30" s="21"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="23"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="B31" s="1">
         <v>3</v>
       </c>
@@ -8989,7 +9380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:14">
       <c r="B32" s="1">
         <v>3</v>
       </c>
@@ -9557,10 +9948,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1479317-8793-42EB-8112-8D25209E1C4C}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9571,33 +9962,37 @@
     <col min="4" max="4" width="25.6875" customWidth="1"/>
     <col min="5" max="5" width="29.125" customWidth="1"/>
     <col min="6" max="6" width="23.6875" customWidth="1"/>
-    <col min="7" max="7" width="21.6875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.4375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -9619,12 +10014,12 @@
         <f>COUNTIF(D:D,A2)</f>
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <f>COUNTIF(E:E, A2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -9646,12 +10041,12 @@
         <f t="shared" ref="F3:F37" si="1">COUNTIF(D:D,A3)</f>
         <v>0</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G37" si="2">COUNTIF(E:E, A3)</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H37" si="2">COUNTIF(E:E, A3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -9673,12 +10068,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -9700,12 +10095,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -9727,12 +10122,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -9754,12 +10149,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -9781,12 +10176,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>0.7</v>
       </c>
@@ -9808,12 +10203,12 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -9835,12 +10230,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -9862,12 +10257,12 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>1</v>
       </c>
@@ -9889,12 +10284,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -9916,12 +10311,12 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -9943,12 +10338,12 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -9970,12 +10365,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -9997,12 +10392,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -10024,12 +10419,12 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -10051,12 +10446,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -10078,12 +10473,12 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -10105,12 +10500,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -10132,12 +10527,12 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>2</v>
       </c>
@@ -10160,11 +10555,14 @@
         <v>1</v>
       </c>
       <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -10186,12 +10584,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -10213,12 +10611,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -10240,12 +10638,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -10267,12 +10665,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -10294,12 +10692,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -10321,12 +10719,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -10348,12 +10746,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -10375,12 +10773,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -10402,12 +10800,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>3</v>
       </c>
@@ -10429,12 +10827,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -10456,12 +10854,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -10483,12 +10881,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -10510,12 +10908,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -10537,12 +10935,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -10564,12 +10962,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8">
       <c r="B38" s="1">
         <v>0.48383599999999999</v>
       </c>
@@ -10585,7 +10983,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="B39" s="1">
         <v>1.4850752</v>
       </c>
@@ -10601,7 +10999,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="B40" s="1">
         <v>0.52325759999999999</v>
       </c>
@@ -10617,7 +11015,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="B41" s="1">
         <v>0.53028370000000002</v>
       </c>
@@ -10633,7 +11031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="B42" s="1">
         <v>0.55262299999999998</v>
       </c>
@@ -10649,7 +11047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="B43" s="1">
         <v>1.5923670000000001</v>
       </c>
@@ -10665,7 +11063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="B44" s="1">
         <v>0.60108019999999995</v>
       </c>
@@ -10681,7 +11079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="B45" s="1">
         <v>0.62007730000000005</v>
       </c>
@@ -10697,7 +11095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="B46" s="1">
         <v>1.6762733999999999</v>
       </c>
@@ -10713,7 +11111,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="B47" s="1">
         <v>0.70408890000000002</v>
       </c>
@@ -10729,7 +11127,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="B48" s="1">
         <v>0.71766490000000005</v>
       </c>
@@ -11632,7 +12030,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>